<commit_message>
refactor: DBRS rating for score 10
Previously, a score of 10 would have been translated into a DBRS
rating of "R-2L / R-3".
Updated screenshots for documentation to reflect a rating of "R-3"
when translating a score of 10 using the base strategy.
</commit_message>
<xml_diff>
--- a/docs/ratings.xlsx
+++ b/docs/ratings.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="143">
   <si>
     <t>C</t>
   </si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t>R-2L</t>
-  </si>
-  <si>
-    <t>R-2L / R-3</t>
   </si>
   <si>
     <t>Rating</t>
@@ -1514,36 +1511,6 @@
     <xf numFmtId="165" fontId="7" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1601,6 +1568,36 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4107,7 +4104,7 @@
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="199" t="s">
+      <c r="B3" s="223" t="s">
         <v>122</v>
       </c>
       <c r="C3" s="192" t="s">
@@ -4128,7 +4125,7 @@
       <c r="H3" s="192">
         <v>1</v>
       </c>
-      <c r="J3" s="199" t="s">
+      <c r="J3" s="223" t="s">
         <v>122</v>
       </c>
       <c r="K3" s="192" t="s">
@@ -4157,7 +4154,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="200"/>
+      <c r="B4" s="224"/>
       <c r="C4" s="38" t="s">
         <v>74</v>
       </c>
@@ -4176,7 +4173,7 @@
       <c r="H4" s="38">
         <v>2</v>
       </c>
-      <c r="J4" s="200"/>
+      <c r="J4" s="224"/>
       <c r="K4" s="38" t="s">
         <v>74</v>
       </c>
@@ -4203,7 +4200,7 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="200"/>
+      <c r="B5" s="224"/>
       <c r="C5" s="37" t="s">
         <v>77</v>
       </c>
@@ -4222,7 +4219,7 @@
       <c r="H5" s="37">
         <v>3</v>
       </c>
-      <c r="J5" s="200"/>
+      <c r="J5" s="224"/>
       <c r="K5" s="37" t="s">
         <v>77</v>
       </c>
@@ -4249,7 +4246,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="200"/>
+      <c r="B6" s="224"/>
       <c r="C6" s="38" t="s">
         <v>79</v>
       </c>
@@ -4268,7 +4265,7 @@
       <c r="H6" s="38">
         <v>4</v>
       </c>
-      <c r="J6" s="200"/>
+      <c r="J6" s="224"/>
       <c r="K6" s="38" t="s">
         <v>79</v>
       </c>
@@ -4295,7 +4292,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="200"/>
+      <c r="B7" s="224"/>
       <c r="C7" s="37" t="s">
         <v>82</v>
       </c>
@@ -4314,7 +4311,7 @@
       <c r="H7" s="37">
         <v>5</v>
       </c>
-      <c r="J7" s="200"/>
+      <c r="J7" s="224"/>
       <c r="K7" s="37" t="s">
         <v>82</v>
       </c>
@@ -4341,7 +4338,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="200"/>
+      <c r="B8" s="224"/>
       <c r="C8" s="38" t="s">
         <v>85</v>
       </c>
@@ -4360,7 +4357,7 @@
       <c r="H8" s="38">
         <v>6</v>
       </c>
-      <c r="J8" s="200"/>
+      <c r="J8" s="224"/>
       <c r="K8" s="38" t="s">
         <v>85</v>
       </c>
@@ -4387,7 +4384,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="200"/>
+      <c r="B9" s="224"/>
       <c r="C9" s="37" t="s">
         <v>87</v>
       </c>
@@ -4406,7 +4403,7 @@
       <c r="H9" s="37">
         <v>7</v>
       </c>
-      <c r="J9" s="200"/>
+      <c r="J9" s="224"/>
       <c r="K9" s="37" t="s">
         <v>87</v>
       </c>
@@ -4433,7 +4430,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="200"/>
+      <c r="B10" s="224"/>
       <c r="C10" s="38" t="s">
         <v>90</v>
       </c>
@@ -4452,7 +4449,7 @@
       <c r="H10" s="38">
         <v>8</v>
       </c>
-      <c r="J10" s="200"/>
+      <c r="J10" s="224"/>
       <c r="K10" s="38" t="s">
         <v>90</v>
       </c>
@@ -4479,7 +4476,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="200"/>
+      <c r="B11" s="224"/>
       <c r="C11" s="37" t="s">
         <v>93</v>
       </c>
@@ -4498,7 +4495,7 @@
       <c r="H11" s="37">
         <v>9</v>
       </c>
-      <c r="J11" s="200"/>
+      <c r="J11" s="224"/>
       <c r="K11" s="37" t="s">
         <v>93</v>
       </c>
@@ -4525,7 +4522,7 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="201"/>
+      <c r="B12" s="225"/>
       <c r="C12" s="39" t="s">
         <v>96</v>
       </c>
@@ -4544,7 +4541,7 @@
       <c r="H12" s="39">
         <v>10</v>
       </c>
-      <c r="J12" s="201"/>
+      <c r="J12" s="225"/>
       <c r="K12" s="39" t="s">
         <v>96</v>
       </c>
@@ -4571,7 +4568,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="199" t="s">
+      <c r="B13" s="223" t="s">
         <v>123</v>
       </c>
       <c r="C13" s="37" t="s">
@@ -4592,7 +4589,7 @@
       <c r="H13" s="37">
         <v>11</v>
       </c>
-      <c r="J13" s="199" t="s">
+      <c r="J13" s="223" t="s">
         <v>123</v>
       </c>
       <c r="K13" s="37" t="s">
@@ -4621,7 +4618,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="200"/>
+      <c r="B14" s="224"/>
       <c r="C14" s="38" t="s">
         <v>102</v>
       </c>
@@ -4640,7 +4637,7 @@
       <c r="H14" s="38">
         <v>12</v>
       </c>
-      <c r="J14" s="200"/>
+      <c r="J14" s="224"/>
       <c r="K14" s="38" t="s">
         <v>102</v>
       </c>
@@ -4667,7 +4664,7 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="200"/>
+      <c r="B15" s="224"/>
       <c r="C15" s="37" t="s">
         <v>104</v>
       </c>
@@ -4686,7 +4683,7 @@
       <c r="H15" s="37">
         <v>13</v>
       </c>
-      <c r="J15" s="200"/>
+      <c r="J15" s="224"/>
       <c r="K15" s="37" t="s">
         <v>104</v>
       </c>
@@ -4713,7 +4710,7 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="200"/>
+      <c r="B16" s="224"/>
       <c r="C16" s="38" t="s">
         <v>107</v>
       </c>
@@ -4732,7 +4729,7 @@
       <c r="H16" s="38">
         <v>14</v>
       </c>
-      <c r="J16" s="200"/>
+      <c r="J16" s="224"/>
       <c r="K16" s="38" t="s">
         <v>107</v>
       </c>
@@ -4759,7 +4756,7 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="200"/>
+      <c r="B17" s="224"/>
       <c r="C17" s="37" t="s">
         <v>110</v>
       </c>
@@ -4778,7 +4775,7 @@
       <c r="H17" s="37">
         <v>15</v>
       </c>
-      <c r="J17" s="200"/>
+      <c r="J17" s="224"/>
       <c r="K17" s="37" t="s">
         <v>110</v>
       </c>
@@ -4805,7 +4802,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="200"/>
+      <c r="B18" s="224"/>
       <c r="C18" s="38" t="s">
         <v>111</v>
       </c>
@@ -4824,7 +4821,7 @@
       <c r="H18" s="38">
         <v>16</v>
       </c>
-      <c r="J18" s="200"/>
+      <c r="J18" s="224"/>
       <c r="K18" s="38" t="s">
         <v>111</v>
       </c>
@@ -4851,7 +4848,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="200"/>
+      <c r="B19" s="224"/>
       <c r="C19" s="37" t="s">
         <v>114</v>
       </c>
@@ -4870,7 +4867,7 @@
       <c r="H19" s="37">
         <v>17</v>
       </c>
-      <c r="J19" s="200"/>
+      <c r="J19" s="224"/>
       <c r="K19" s="37" t="s">
         <v>114</v>
       </c>
@@ -4897,7 +4894,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="200"/>
+      <c r="B20" s="224"/>
       <c r="C20" s="38" t="s">
         <v>117</v>
       </c>
@@ -4916,7 +4913,7 @@
       <c r="H20" s="38">
         <v>18</v>
       </c>
-      <c r="J20" s="200"/>
+      <c r="J20" s="224"/>
       <c r="K20" s="38" t="s">
         <v>117</v>
       </c>
@@ -4943,7 +4940,7 @@
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="200"/>
+      <c r="B21" s="224"/>
       <c r="C21" s="37" t="s">
         <v>118</v>
       </c>
@@ -4962,7 +4959,7 @@
       <c r="H21" s="37">
         <v>19</v>
       </c>
-      <c r="J21" s="200"/>
+      <c r="J21" s="224"/>
       <c r="K21" s="37" t="s">
         <v>118</v>
       </c>
@@ -4989,7 +4986,7 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="200"/>
+      <c r="B22" s="224"/>
       <c r="C22" s="38" t="s">
         <v>120</v>
       </c>
@@ -5008,7 +5005,7 @@
       <c r="H22" s="38">
         <v>20</v>
       </c>
-      <c r="J22" s="200"/>
+      <c r="J22" s="224"/>
       <c r="K22" s="38" t="s">
         <v>120</v>
       </c>
@@ -5035,7 +5032,7 @@
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="200"/>
+      <c r="B23" s="224"/>
       <c r="C23" s="37" t="s">
         <v>0</v>
       </c>
@@ -5054,7 +5051,7 @@
       <c r="H23" s="37">
         <v>21</v>
       </c>
-      <c r="J23" s="200"/>
+      <c r="J23" s="224"/>
       <c r="K23" s="37" t="s">
         <v>0</v>
       </c>
@@ -5081,7 +5078,7 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="201"/>
+      <c r="B24" s="225"/>
       <c r="C24" s="39" t="s">
         <v>125</v>
       </c>
@@ -5100,7 +5097,7 @@
       <c r="H24" s="39">
         <v>22</v>
       </c>
-      <c r="J24" s="201"/>
+      <c r="J24" s="225"/>
       <c r="K24" s="39" t="s">
         <v>1</v>
       </c>
@@ -5127,24 +5124,24 @@
       </c>
     </row>
     <row r="25" spans="2:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="202" t="s">
+      <c r="B25" s="226" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="202"/>
-      <c r="D25" s="202"/>
-      <c r="E25" s="202"/>
-      <c r="F25" s="202"/>
-      <c r="G25" s="202"/>
-      <c r="H25" s="202"/>
-      <c r="J25" s="203" t="s">
+      <c r="C25" s="226"/>
+      <c r="D25" s="226"/>
+      <c r="E25" s="226"/>
+      <c r="F25" s="226"/>
+      <c r="G25" s="226"/>
+      <c r="H25" s="226"/>
+      <c r="J25" s="227" t="s">
         <v>135</v>
       </c>
-      <c r="K25" s="203"/>
-      <c r="L25" s="203"/>
-      <c r="M25" s="203"/>
-      <c r="N25" s="203"/>
-      <c r="O25" s="203"/>
-      <c r="P25" s="203"/>
+      <c r="K25" s="227"/>
+      <c r="L25" s="227"/>
+      <c r="M25" s="227"/>
+      <c r="N25" s="227"/>
+      <c r="O25" s="227"/>
+      <c r="P25" s="227"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5169,8 +5166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:CZ83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BD88" sqref="BD88"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CH18" sqref="CH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5263,13 +5260,13 @@
         <v>44</v>
       </c>
       <c r="BD2" s="121" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BE2" s="122" t="s">
         <v>71</v>
       </c>
       <c r="BF2" s="131" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BG2" s="131" t="s">
         <v>65</v>
@@ -5278,7 +5275,7 @@
         <v>66</v>
       </c>
       <c r="BI2" s="132" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BK2" s="121" t="s">
         <v>64</v>
@@ -5436,22 +5433,22 @@
       <c r="AZ3" s="78"/>
       <c r="BA3" s="79"/>
       <c r="BB3" s="34"/>
-      <c r="BD3" s="217" t="s">
+      <c r="BD3" s="207" t="s">
         <v>2</v>
       </c>
-      <c r="BE3" s="218" t="s">
+      <c r="BE3" s="208" t="s">
         <v>60</v>
       </c>
-      <c r="BF3" s="219" t="s">
+      <c r="BF3" s="209" t="s">
         <v>5</v>
       </c>
-      <c r="BG3" s="219">
+      <c r="BG3" s="209">
         <v>1</v>
       </c>
-      <c r="BH3" s="219">
+      <c r="BH3" s="209">
         <v>7</v>
       </c>
-      <c r="BI3" s="220">
+      <c r="BI3" s="210">
         <f>AVERAGE(BG3:BH3)</f>
         <v>4</v>
       </c>
@@ -5542,7 +5539,7 @@
         <v>50</v>
       </c>
       <c r="CS3" s="2"/>
-      <c r="CT3" s="204" t="s">
+      <c r="CT3" s="228" t="s">
         <v>51</v>
       </c>
       <c r="CU3" s="2"/>
@@ -5657,16 +5654,16 @@
       <c r="BE4" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF4" s="211" t="s">
+      <c r="BF4" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="BG4" s="211">
+      <c r="BG4" s="201">
         <v>8</v>
       </c>
-      <c r="BH4" s="211">
+      <c r="BH4" s="201">
         <v>9</v>
       </c>
-      <c r="BI4" s="212">
+      <c r="BI4" s="202">
         <f t="shared" ref="BI4:BI6" si="3">AVERAGE(BG4:BH4)</f>
         <v>8.5</v>
       </c>
@@ -5747,7 +5744,7 @@
         <v>4.5</v>
       </c>
       <c r="CM4" s="2"/>
-      <c r="CN4" s="206" t="s">
+      <c r="CN4" s="230" t="s">
         <v>52</v>
       </c>
       <c r="CO4" s="58" t="s">
@@ -5762,7 +5759,7 @@
         <v>3.5</v>
       </c>
       <c r="CS4" s="60"/>
-      <c r="CT4" s="205"/>
+      <c r="CT4" s="229"/>
       <c r="CU4" s="60"/>
       <c r="CV4" s="60"/>
       <c r="CW4" s="2"/>
@@ -5888,19 +5885,19 @@
       <c r="BD5" s="155" t="s">
         <v>2</v>
       </c>
-      <c r="BE5" s="228" t="s">
+      <c r="BE5" s="218" t="s">
         <v>60</v>
       </c>
-      <c r="BF5" s="222" t="s">
+      <c r="BF5" s="212" t="s">
         <v>7</v>
       </c>
-      <c r="BG5" s="222">
+      <c r="BG5" s="212">
         <v>10</v>
       </c>
-      <c r="BH5" s="222">
+      <c r="BH5" s="212">
         <v>10</v>
       </c>
-      <c r="BI5" s="223">
+      <c r="BI5" s="213">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -5981,7 +5978,7 @@
         <v>7</v>
       </c>
       <c r="CM5" s="2"/>
-      <c r="CN5" s="207"/>
+      <c r="CN5" s="231"/>
       <c r="CO5" s="61" t="s">
         <v>9</v>
       </c>
@@ -6128,16 +6125,16 @@
       <c r="BE6" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF6" s="211" t="s">
+      <c r="BF6" s="201" t="s">
         <v>8</v>
       </c>
-      <c r="BG6" s="211">
+      <c r="BG6" s="201">
         <v>11</v>
       </c>
-      <c r="BH6" s="211">
+      <c r="BH6" s="201">
         <v>22</v>
       </c>
-      <c r="BI6" s="212">
+      <c r="BI6" s="202">
         <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
@@ -6218,7 +6215,7 @@
         <v>9</v>
       </c>
       <c r="CM6" s="2"/>
-      <c r="CN6" s="208"/>
+      <c r="CN6" s="232"/>
       <c r="CO6" s="65" t="s">
         <v>10</v>
       </c>
@@ -6234,7 +6231,7 @@
       <c r="CT6" s="60"/>
       <c r="CU6" s="60"/>
       <c r="CV6" s="64"/>
-      <c r="CW6" s="204" t="s">
+      <c r="CW6" s="228" t="s">
         <v>53</v>
       </c>
       <c r="CX6" s="2"/>
@@ -6360,22 +6357,22 @@
       <c r="BB7" s="18">
         <v>3</v>
       </c>
-      <c r="BD7" s="224" t="s">
+      <c r="BD7" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="BE7" s="225" t="s">
+      <c r="BE7" s="215" t="s">
         <v>70</v>
       </c>
-      <c r="BF7" s="226" t="s">
+      <c r="BF7" s="216" t="s">
         <v>5</v>
       </c>
-      <c r="BG7" s="226">
+      <c r="BG7" s="216">
         <v>1</v>
       </c>
-      <c r="BH7" s="226">
+      <c r="BH7" s="216">
         <v>6</v>
       </c>
-      <c r="BI7" s="227">
+      <c r="BI7" s="217">
         <f>AVERAGE(BG7:BH7)</f>
         <v>3.5</v>
       </c>
@@ -6465,7 +6462,7 @@
       <c r="CT7" s="60"/>
       <c r="CU7" s="60"/>
       <c r="CV7" s="64"/>
-      <c r="CW7" s="205"/>
+      <c r="CW7" s="229"/>
       <c r="CX7" s="2"/>
       <c r="CY7" s="55" t="s">
         <v>6</v>
@@ -6595,16 +6592,16 @@
       <c r="BE8" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF8" s="211" t="s">
+      <c r="BF8" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="BG8" s="211">
+      <c r="BG8" s="201">
         <v>7</v>
       </c>
-      <c r="BH8" s="211">
+      <c r="BH8" s="201">
         <v>8</v>
       </c>
-      <c r="BI8" s="212">
+      <c r="BI8" s="202">
         <f t="shared" ref="BI8:BI10" si="5">AVERAGE(BG8:BH8)</f>
         <v>7.5</v>
       </c>
@@ -6826,19 +6823,19 @@
       <c r="BD9" s="155" t="s">
         <v>2</v>
       </c>
-      <c r="BE9" s="221" t="s">
+      <c r="BE9" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF9" s="222" t="s">
+      <c r="BF9" s="212" t="s">
         <v>7</v>
       </c>
-      <c r="BG9" s="222">
+      <c r="BG9" s="212">
         <v>9</v>
       </c>
-      <c r="BH9" s="222">
+      <c r="BH9" s="212">
         <v>10</v>
       </c>
-      <c r="BI9" s="223">
+      <c r="BI9" s="213">
         <f t="shared" si="5"/>
         <v>9.5</v>
       </c>
@@ -6929,7 +6926,7 @@
         <v>50</v>
       </c>
       <c r="CS9" s="60"/>
-      <c r="CT9" s="204" t="s">
+      <c r="CT9" s="228" t="s">
         <v>51</v>
       </c>
       <c r="CU9" s="60"/>
@@ -7066,16 +7063,16 @@
       <c r="BE10" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF10" s="211" t="s">
+      <c r="BF10" s="201" t="s">
         <v>8</v>
       </c>
-      <c r="BG10" s="211">
+      <c r="BG10" s="201">
         <v>11</v>
       </c>
-      <c r="BH10" s="211">
+      <c r="BH10" s="201">
         <v>22</v>
       </c>
-      <c r="BI10" s="212">
+      <c r="BI10" s="202">
         <f t="shared" si="5"/>
         <v>16.5</v>
       </c>
@@ -7156,7 +7153,7 @@
         <v>18.5</v>
       </c>
       <c r="CM10" s="2"/>
-      <c r="CN10" s="206" t="s">
+      <c r="CN10" s="230" t="s">
         <v>56</v>
       </c>
       <c r="CO10" s="58" t="s">
@@ -7171,7 +7168,7 @@
         <v>7.5</v>
       </c>
       <c r="CS10" s="60"/>
-      <c r="CT10" s="205"/>
+      <c r="CT10" s="229"/>
       <c r="CU10" s="60"/>
       <c r="CV10" s="64"/>
       <c r="CW10" s="71">
@@ -7303,22 +7300,22 @@
       <c r="BB11" s="18">
         <v>7</v>
       </c>
-      <c r="BD11" s="224" t="s">
+      <c r="BD11" s="214" t="s">
         <v>2</v>
       </c>
-      <c r="BE11" s="225" t="s">
+      <c r="BE11" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="BF11" s="226" t="s">
+      <c r="BF11" s="216" t="s">
         <v>5</v>
       </c>
-      <c r="BG11" s="226">
+      <c r="BG11" s="216">
         <v>1</v>
       </c>
-      <c r="BH11" s="226">
+      <c r="BH11" s="216">
         <v>5</v>
       </c>
-      <c r="BI11" s="227">
+      <c r="BI11" s="217">
         <f>AVERAGE(BG11:BH11)</f>
         <v>3</v>
       </c>
@@ -7399,7 +7396,7 @@
         <v>22</v>
       </c>
       <c r="CM11" s="2"/>
-      <c r="CN11" s="207"/>
+      <c r="CN11" s="231"/>
       <c r="CO11" s="61" t="s">
         <v>9</v>
       </c>
@@ -7542,16 +7539,16 @@
       <c r="BE12" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF12" s="211" t="s">
+      <c r="BF12" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="BG12" s="211">
+      <c r="BG12" s="201">
         <v>6</v>
       </c>
-      <c r="BH12" s="211">
+      <c r="BH12" s="201">
         <v>8</v>
       </c>
-      <c r="BI12" s="212">
+      <c r="BI12" s="202">
         <f t="shared" ref="BI12:BI75" si="7">AVERAGE(BG12:BH12)</f>
         <v>7</v>
       </c>
@@ -7632,7 +7629,7 @@
         <v>1.5</v>
       </c>
       <c r="CM12" s="2"/>
-      <c r="CN12" s="208"/>
+      <c r="CN12" s="232"/>
       <c r="CO12" s="65" t="s">
         <v>10</v>
       </c>
@@ -7771,19 +7768,19 @@
       <c r="BD13" s="155" t="s">
         <v>2</v>
       </c>
-      <c r="BE13" s="221" t="s">
+      <c r="BE13" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF13" s="222" t="s">
+      <c r="BF13" s="212" t="s">
         <v>7</v>
       </c>
-      <c r="BG13" s="222">
+      <c r="BG13" s="212">
         <v>9</v>
       </c>
-      <c r="BH13" s="222">
+      <c r="BH13" s="212">
         <v>10</v>
       </c>
-      <c r="BI13" s="223">
+      <c r="BI13" s="213">
         <f t="shared" si="7"/>
         <v>9.5</v>
       </c>
@@ -7938,7 +7935,7 @@
         <v>20</v>
       </c>
       <c r="AG14" s="172" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="AI14" s="165"/>
       <c r="AJ14" s="165"/>
@@ -7983,7 +7980,7 @@
         <v>63</v>
       </c>
       <c r="AZ14" s="100" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="BA14" s="101" t="s">
         <v>45</v>
@@ -7997,16 +7994,16 @@
       <c r="BE14" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="BF14" s="215" t="s">
+      <c r="BF14" s="205" t="s">
         <v>8</v>
       </c>
-      <c r="BG14" s="215">
+      <c r="BG14" s="205">
         <v>11</v>
       </c>
-      <c r="BH14" s="215">
+      <c r="BH14" s="205">
         <v>22</v>
       </c>
-      <c r="BI14" s="216">
+      <c r="BI14" s="206">
         <f t="shared" si="7"/>
         <v>16.5</v>
       </c>
@@ -8197,22 +8194,22 @@
       <c r="BB15" s="18">
         <v>11</v>
       </c>
-      <c r="BD15" s="217" t="s">
+      <c r="BD15" s="207" t="s">
         <v>9</v>
       </c>
-      <c r="BE15" s="218" t="s">
+      <c r="BE15" s="208" t="s">
         <v>60</v>
       </c>
-      <c r="BF15" s="219" t="s">
+      <c r="BF15" s="209" t="s">
         <v>12</v>
       </c>
-      <c r="BG15" s="219">
+      <c r="BG15" s="209">
         <v>1</v>
       </c>
-      <c r="BH15" s="219">
+      <c r="BH15" s="209">
         <v>5</v>
       </c>
-      <c r="BI15" s="220">
+      <c r="BI15" s="210">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
@@ -8386,16 +8383,16 @@
       <c r="BE16" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF16" s="211" t="s">
+      <c r="BF16" s="201" t="s">
         <v>13</v>
       </c>
-      <c r="BG16" s="211">
+      <c r="BG16" s="201">
         <v>6</v>
       </c>
-      <c r="BH16" s="211">
+      <c r="BH16" s="201">
         <v>7</v>
       </c>
-      <c r="BI16" s="212">
+      <c r="BI16" s="202">
         <f t="shared" si="7"/>
         <v>6.5</v>
       </c>
@@ -8578,19 +8575,19 @@
       <c r="BD17" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE17" s="221" t="s">
+      <c r="BE17" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF17" s="222" t="s">
+      <c r="BF17" s="212" t="s">
         <v>14</v>
       </c>
-      <c r="BG17" s="222">
+      <c r="BG17" s="212">
         <v>8</v>
       </c>
-      <c r="BH17" s="222">
+      <c r="BH17" s="212">
         <v>9</v>
       </c>
-      <c r="BI17" s="223">
+      <c r="BI17" s="213">
         <f t="shared" si="7"/>
         <v>8.5</v>
       </c>
@@ -8639,7 +8636,7 @@
         <v>70</v>
       </c>
       <c r="CH17" s="100" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="CI17" s="100">
         <v>10</v>
@@ -8662,7 +8659,7 @@
         <v>50</v>
       </c>
       <c r="CS17" s="2"/>
-      <c r="CT17" s="204" t="s">
+      <c r="CT17" s="228" t="s">
         <v>51</v>
       </c>
       <c r="CU17" s="2"/>
@@ -8782,16 +8779,16 @@
       <c r="BE18" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF18" s="211" t="s">
+      <c r="BF18" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="BG18" s="211">
+      <c r="BG18" s="201">
         <v>10</v>
       </c>
-      <c r="BH18" s="211">
+      <c r="BH18" s="201">
         <v>11</v>
       </c>
-      <c r="BI18" s="212">
+      <c r="BI18" s="202">
         <f t="shared" si="7"/>
         <v>10.5</v>
       </c>
@@ -8853,7 +8850,7 @@
         <v>12.5</v>
       </c>
       <c r="CM18" s="2"/>
-      <c r="CN18" s="206" t="s">
+      <c r="CN18" s="230" t="s">
         <v>52</v>
       </c>
       <c r="CO18" s="58" t="s">
@@ -8867,7 +8864,7 @@
         <v>1</v>
       </c>
       <c r="CS18" s="60"/>
-      <c r="CT18" s="205"/>
+      <c r="CT18" s="229"/>
       <c r="CU18" s="60"/>
       <c r="CV18" s="60"/>
       <c r="CW18" s="2"/>
@@ -8984,19 +8981,19 @@
       <c r="BD19" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE19" s="221" t="s">
+      <c r="BE19" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF19" s="222" t="s">
+      <c r="BF19" s="212" t="s">
         <v>16</v>
       </c>
-      <c r="BG19" s="222">
+      <c r="BG19" s="212">
         <v>12</v>
       </c>
-      <c r="BH19" s="222">
+      <c r="BH19" s="212">
         <v>16</v>
       </c>
-      <c r="BI19" s="223">
+      <c r="BI19" s="213">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
@@ -9058,7 +9055,7 @@
         <v>18</v>
       </c>
       <c r="CM19" s="2"/>
-      <c r="CN19" s="207"/>
+      <c r="CN19" s="231"/>
       <c r="CO19" s="61" t="s">
         <v>9</v>
       </c>
@@ -9191,16 +9188,16 @@
       <c r="BE20" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF20" s="211" t="s">
+      <c r="BF20" s="201" t="s">
         <v>0</v>
       </c>
-      <c r="BG20" s="211">
+      <c r="BG20" s="201">
         <v>17</v>
       </c>
-      <c r="BH20" s="211">
+      <c r="BH20" s="201">
         <v>21</v>
       </c>
-      <c r="BI20" s="212">
+      <c r="BI20" s="202">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
@@ -9262,7 +9259,7 @@
         <v>22</v>
       </c>
       <c r="CM20" s="2"/>
-      <c r="CN20" s="208"/>
+      <c r="CN20" s="232"/>
       <c r="CO20" s="65" t="s">
         <v>10</v>
       </c>
@@ -9277,7 +9274,7 @@
       <c r="CT20" s="60"/>
       <c r="CU20" s="60"/>
       <c r="CV20" s="64"/>
-      <c r="CW20" s="204" t="s">
+      <c r="CW20" s="228" t="s">
         <v>53</v>
       </c>
       <c r="CX20" s="2"/>
@@ -9393,19 +9390,19 @@
       <c r="BD21" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE21" s="221" t="s">
+      <c r="BE21" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF21" s="222" t="s">
+      <c r="BF21" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="BG21" s="222">
+      <c r="BG21" s="212">
         <v>22</v>
       </c>
-      <c r="BH21" s="222">
+      <c r="BH21" s="212">
         <v>22</v>
       </c>
-      <c r="BI21" s="223">
+      <c r="BI21" s="213">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
@@ -9476,7 +9473,7 @@
       <c r="CT21" s="60"/>
       <c r="CU21" s="60"/>
       <c r="CV21" s="64"/>
-      <c r="CW21" s="205"/>
+      <c r="CW21" s="229"/>
       <c r="CX21" s="2"/>
       <c r="CY21" s="55" t="s">
         <v>6</v>
@@ -9593,16 +9590,16 @@
       <c r="BE22" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="BF22" s="213" t="s">
+      <c r="BF22" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="BG22" s="213">
+      <c r="BG22" s="203">
         <v>1</v>
       </c>
-      <c r="BH22" s="213">
+      <c r="BH22" s="203">
         <v>4</v>
       </c>
-      <c r="BI22" s="214">
+      <c r="BI22" s="204">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
@@ -9790,19 +9787,19 @@
       <c r="BD23" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE23" s="221" t="s">
+      <c r="BE23" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF23" s="222" t="s">
+      <c r="BF23" s="212" t="s">
         <v>13</v>
       </c>
-      <c r="BG23" s="222">
+      <c r="BG23" s="212">
         <v>5</v>
       </c>
-      <c r="BH23" s="222">
+      <c r="BH23" s="212">
         <v>6</v>
       </c>
-      <c r="BI23" s="223">
+      <c r="BI23" s="213">
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
@@ -9874,7 +9871,7 @@
         <v>50</v>
       </c>
       <c r="CS23" s="60"/>
-      <c r="CT23" s="204" t="s">
+      <c r="CT23" s="228" t="s">
         <v>51</v>
       </c>
       <c r="CU23" s="60"/>
@@ -9998,16 +9995,16 @@
       <c r="BE24" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF24" s="211" t="s">
+      <c r="BF24" s="201" t="s">
         <v>14</v>
       </c>
-      <c r="BG24" s="211">
+      <c r="BG24" s="201">
         <v>7</v>
       </c>
-      <c r="BH24" s="211">
+      <c r="BH24" s="201">
         <v>9</v>
       </c>
-      <c r="BI24" s="212">
+      <c r="BI24" s="202">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
@@ -10031,7 +10028,7 @@
         <v>7.5</v>
       </c>
       <c r="CM24" s="2"/>
-      <c r="CN24" s="206" t="s">
+      <c r="CN24" s="230" t="s">
         <v>56</v>
       </c>
       <c r="CO24" s="58" t="s">
@@ -10045,7 +10042,7 @@
         <v>7</v>
       </c>
       <c r="CS24" s="60"/>
-      <c r="CT24" s="205"/>
+      <c r="CT24" s="229"/>
       <c r="CU24" s="60"/>
       <c r="CV24" s="64"/>
       <c r="CW24" s="71">
@@ -10163,19 +10160,19 @@
       <c r="BD25" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE25" s="221" t="s">
+      <c r="BE25" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF25" s="222" t="s">
+      <c r="BF25" s="212" t="s">
         <v>15</v>
       </c>
-      <c r="BG25" s="222">
+      <c r="BG25" s="212">
         <v>10</v>
       </c>
-      <c r="BH25" s="222">
+      <c r="BH25" s="212">
         <v>10</v>
       </c>
-      <c r="BI25" s="223">
+      <c r="BI25" s="213">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
@@ -10199,7 +10196,7 @@
         <v>9</v>
       </c>
       <c r="CM25" s="2"/>
-      <c r="CN25" s="207"/>
+      <c r="CN25" s="231"/>
       <c r="CO25" s="61" t="s">
         <v>9</v>
       </c>
@@ -10332,16 +10329,16 @@
       <c r="BE26" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF26" s="211" t="s">
+      <c r="BF26" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="BG26" s="211">
+      <c r="BG26" s="201">
         <v>11</v>
       </c>
-      <c r="BH26" s="211">
+      <c r="BH26" s="201">
         <v>16</v>
       </c>
-      <c r="BI26" s="212">
+      <c r="BI26" s="202">
         <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
@@ -10365,7 +10362,7 @@
         <v>10</v>
       </c>
       <c r="CM26" s="2"/>
-      <c r="CN26" s="208"/>
+      <c r="CN26" s="232"/>
       <c r="CO26" s="65" t="s">
         <v>10</v>
       </c>
@@ -10397,19 +10394,19 @@
       <c r="BD27" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE27" s="221" t="s">
+      <c r="BE27" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF27" s="222" t="s">
+      <c r="BF27" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="BG27" s="222">
+      <c r="BG27" s="212">
         <v>17</v>
       </c>
-      <c r="BH27" s="222">
+      <c r="BH27" s="212">
         <v>21</v>
       </c>
-      <c r="BI27" s="223">
+      <c r="BI27" s="213">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
@@ -10455,16 +10452,16 @@
       <c r="BE28" s="127" t="s">
         <v>70</v>
       </c>
-      <c r="BF28" s="215" t="s">
+      <c r="BF28" s="205" t="s">
         <v>1</v>
       </c>
-      <c r="BG28" s="215">
+      <c r="BG28" s="205">
         <v>22</v>
       </c>
-      <c r="BH28" s="215">
+      <c r="BH28" s="205">
         <v>22</v>
       </c>
-      <c r="BI28" s="216">
+      <c r="BI28" s="206">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
@@ -10510,19 +10507,19 @@
       <c r="BD29" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE29" s="221" t="s">
+      <c r="BE29" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF29" s="222" t="s">
+      <c r="BF29" s="212" t="s">
         <v>12</v>
       </c>
-      <c r="BG29" s="222">
+      <c r="BG29" s="212">
         <v>1</v>
       </c>
-      <c r="BH29" s="222">
+      <c r="BH29" s="212">
         <v>4</v>
       </c>
-      <c r="BI29" s="223">
+      <c r="BI29" s="213">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
@@ -10572,16 +10569,16 @@
       <c r="BE30" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF30" s="211" t="s">
+      <c r="BF30" s="201" t="s">
         <v>13</v>
       </c>
-      <c r="BG30" s="211">
+      <c r="BG30" s="201">
         <v>5</v>
       </c>
-      <c r="BH30" s="211">
+      <c r="BH30" s="201">
         <v>6</v>
       </c>
-      <c r="BI30" s="212">
+      <c r="BI30" s="202">
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
@@ -10608,19 +10605,19 @@
       <c r="BD31" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE31" s="221" t="s">
+      <c r="BE31" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF31" s="222" t="s">
+      <c r="BF31" s="212" t="s">
         <v>14</v>
       </c>
-      <c r="BG31" s="222">
+      <c r="BG31" s="212">
         <v>7</v>
       </c>
-      <c r="BH31" s="222">
+      <c r="BH31" s="212">
         <v>9</v>
       </c>
-      <c r="BI31" s="223">
+      <c r="BI31" s="213">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
@@ -10658,16 +10655,16 @@
       <c r="BE32" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF32" s="211" t="s">
+      <c r="BF32" s="201" t="s">
         <v>15</v>
       </c>
-      <c r="BG32" s="211">
+      <c r="BG32" s="201">
         <v>10</v>
       </c>
-      <c r="BH32" s="211">
+      <c r="BH32" s="201">
         <v>10</v>
       </c>
-      <c r="BI32" s="212">
+      <c r="BI32" s="202">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
@@ -10688,19 +10685,19 @@
       <c r="BD33" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="BE33" s="221" t="s">
+      <c r="BE33" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF33" s="222" t="s">
+      <c r="BF33" s="212" t="s">
         <v>16</v>
       </c>
-      <c r="BG33" s="222">
+      <c r="BG33" s="212">
         <v>11</v>
       </c>
-      <c r="BH33" s="222">
+      <c r="BH33" s="212">
         <v>16</v>
       </c>
-      <c r="BI33" s="223">
+      <c r="BI33" s="213">
         <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
@@ -10714,7 +10711,7 @@
         <v>50</v>
       </c>
       <c r="CS33" s="2"/>
-      <c r="CT33" s="204" t="s">
+      <c r="CT33" s="228" t="s">
         <v>51</v>
       </c>
       <c r="CU33" s="2"/>
@@ -10742,20 +10739,20 @@
       <c r="BE34" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF34" s="211" t="s">
+      <c r="BF34" s="201" t="s">
         <v>0</v>
       </c>
-      <c r="BG34" s="211">
+      <c r="BG34" s="201">
         <v>17</v>
       </c>
-      <c r="BH34" s="211">
+      <c r="BH34" s="201">
         <v>21</v>
       </c>
-      <c r="BI34" s="212">
+      <c r="BI34" s="202">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="CN34" s="206" t="s">
+      <c r="CN34" s="230" t="s">
         <v>52</v>
       </c>
       <c r="CO34" s="58" t="s">
@@ -10769,7 +10766,7 @@
         <v>6</v>
       </c>
       <c r="CS34" s="60"/>
-      <c r="CT34" s="205"/>
+      <c r="CT34" s="229"/>
       <c r="CU34" s="60"/>
       <c r="CV34" s="60"/>
       <c r="CW34" s="2"/>
@@ -10789,26 +10786,26 @@
       <c r="Z35" s="1"/>
       <c r="AG35" s="1"/>
       <c r="AL35" s="1"/>
-      <c r="BD35" s="229" t="s">
+      <c r="BD35" s="219" t="s">
         <v>9</v>
       </c>
-      <c r="BE35" s="230" t="s">
+      <c r="BE35" s="220" t="s">
         <v>61</v>
       </c>
-      <c r="BF35" s="231" t="s">
+      <c r="BF35" s="221" t="s">
         <v>1</v>
       </c>
-      <c r="BG35" s="231">
+      <c r="BG35" s="221">
         <v>22</v>
       </c>
-      <c r="BH35" s="231">
+      <c r="BH35" s="221">
         <v>22</v>
       </c>
-      <c r="BI35" s="232">
+      <c r="BI35" s="222">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="CN35" s="207"/>
+      <c r="CN35" s="231"/>
       <c r="CO35" s="61" t="s">
         <v>9</v>
       </c>
@@ -10849,20 +10846,20 @@
       <c r="BE36" s="124" t="s">
         <v>60</v>
       </c>
-      <c r="BF36" s="209" t="s">
+      <c r="BF36" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="BG36" s="209">
+      <c r="BG36" s="199">
         <v>1</v>
       </c>
-      <c r="BH36" s="209">
+      <c r="BH36" s="199">
         <v>6</v>
       </c>
-      <c r="BI36" s="210">
+      <c r="BI36" s="200">
         <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
-      <c r="CN36" s="208"/>
+      <c r="CN36" s="232"/>
       <c r="CO36" s="65" t="s">
         <v>10</v>
       </c>
@@ -10877,7 +10874,7 @@
       <c r="CT36" s="60"/>
       <c r="CU36" s="60"/>
       <c r="CV36" s="64"/>
-      <c r="CW36" s="204" t="s">
+      <c r="CW36" s="228" t="s">
         <v>53</v>
       </c>
       <c r="CX36" s="2"/>
@@ -10901,19 +10898,19 @@
       <c r="BD37" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE37" s="221" t="s">
+      <c r="BE37" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF37" s="222" t="s">
+      <c r="BF37" s="212" t="s">
         <v>18</v>
       </c>
-      <c r="BG37" s="222">
+      <c r="BG37" s="212">
         <v>7</v>
       </c>
-      <c r="BH37" s="222">
+      <c r="BH37" s="212">
         <v>8</v>
       </c>
-      <c r="BI37" s="223">
+      <c r="BI37" s="213">
         <f t="shared" si="7"/>
         <v>7.5</v>
       </c>
@@ -10926,7 +10923,7 @@
       <c r="CT37" s="60"/>
       <c r="CU37" s="60"/>
       <c r="CV37" s="64"/>
-      <c r="CW37" s="205"/>
+      <c r="CW37" s="229"/>
       <c r="CX37" s="2"/>
       <c r="CY37" s="55" t="s">
         <v>6</v>
@@ -10951,16 +10948,16 @@
       <c r="BE38" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF38" s="211" t="s">
+      <c r="BF38" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="BG38" s="211">
+      <c r="BG38" s="201">
         <v>9</v>
       </c>
-      <c r="BH38" s="211">
+      <c r="BH38" s="201">
         <v>9</v>
       </c>
-      <c r="BI38" s="212">
+      <c r="BI38" s="202">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
@@ -10998,19 +10995,19 @@
       <c r="BD39" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE39" s="221" t="s">
+      <c r="BE39" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF39" s="222" t="s">
+      <c r="BF39" s="212" t="s">
         <v>20</v>
       </c>
-      <c r="BG39" s="222">
+      <c r="BG39" s="212">
         <v>10</v>
       </c>
-      <c r="BH39" s="222">
+      <c r="BH39" s="212">
         <v>10</v>
       </c>
-      <c r="BI39" s="223">
+      <c r="BI39" s="213">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
@@ -11024,7 +11021,7 @@
         <v>50</v>
       </c>
       <c r="CS39" s="60"/>
-      <c r="CT39" s="204" t="s">
+      <c r="CT39" s="228" t="s">
         <v>51</v>
       </c>
       <c r="CU39" s="60"/>
@@ -11056,20 +11053,20 @@
       <c r="BE40" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF40" s="211" t="s">
+      <c r="BF40" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="BG40" s="211">
+      <c r="BG40" s="201">
         <v>11</v>
       </c>
-      <c r="BH40" s="211">
+      <c r="BH40" s="201">
         <v>16</v>
       </c>
-      <c r="BI40" s="212">
+      <c r="BI40" s="202">
         <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
-      <c r="CN40" s="206" t="s">
+      <c r="CN40" s="230" t="s">
         <v>56</v>
       </c>
       <c r="CO40" s="58" t="s">
@@ -11083,7 +11080,7 @@
         <v>8</v>
       </c>
       <c r="CS40" s="60"/>
-      <c r="CT40" s="205"/>
+      <c r="CT40" s="229"/>
       <c r="CU40" s="60"/>
       <c r="CV40" s="64"/>
       <c r="CW40" s="71">
@@ -11109,23 +11106,23 @@
       <c r="BD41" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE41" s="221" t="s">
+      <c r="BE41" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF41" s="222" t="s">
+      <c r="BF41" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="BG41" s="222">
+      <c r="BG41" s="212">
         <v>17</v>
       </c>
-      <c r="BH41" s="222">
+      <c r="BH41" s="212">
         <v>20</v>
       </c>
-      <c r="BI41" s="223">
+      <c r="BI41" s="213">
         <f t="shared" si="7"/>
         <v>18.5</v>
       </c>
-      <c r="CN41" s="207"/>
+      <c r="CN41" s="231"/>
       <c r="CO41" s="61" t="s">
         <v>9</v>
       </c>
@@ -11165,20 +11162,20 @@
       <c r="BE42" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF42" s="211" t="s">
+      <c r="BF42" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="BG42" s="211">
+      <c r="BG42" s="201">
         <v>21</v>
       </c>
-      <c r="BH42" s="211">
+      <c r="BH42" s="201">
         <v>22</v>
       </c>
-      <c r="BI42" s="212">
+      <c r="BI42" s="202">
         <f t="shared" si="7"/>
         <v>21.5</v>
       </c>
-      <c r="CN42" s="208"/>
+      <c r="CN42" s="232"/>
       <c r="CO42" s="65" t="s">
         <v>10</v>
       </c>
@@ -11209,22 +11206,22 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
       <c r="AG43" s="1"/>
-      <c r="BD43" s="224" t="s">
+      <c r="BD43" s="214" t="s">
         <v>10</v>
       </c>
-      <c r="BE43" s="225" t="s">
+      <c r="BE43" s="215" t="s">
         <v>70</v>
       </c>
-      <c r="BF43" s="226" t="s">
+      <c r="BF43" s="216" t="s">
         <v>17</v>
       </c>
-      <c r="BG43" s="226">
+      <c r="BG43" s="216">
         <v>1</v>
       </c>
-      <c r="BH43" s="226">
+      <c r="BH43" s="216">
         <v>5</v>
       </c>
-      <c r="BI43" s="227">
+      <c r="BI43" s="217">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
@@ -11247,16 +11244,16 @@
       <c r="BE44" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF44" s="211" t="s">
+      <c r="BF44" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="BG44" s="211">
+      <c r="BG44" s="201">
         <v>6</v>
       </c>
-      <c r="BH44" s="211">
+      <c r="BH44" s="201">
         <v>7</v>
       </c>
-      <c r="BI44" s="212">
+      <c r="BI44" s="202">
         <f t="shared" si="7"/>
         <v>6.5</v>
       </c>
@@ -11276,19 +11273,19 @@
       <c r="BD45" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE45" s="221" t="s">
+      <c r="BE45" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF45" s="222" t="s">
+      <c r="BF45" s="212" t="s">
         <v>19</v>
       </c>
-      <c r="BG45" s="222">
+      <c r="BG45" s="212">
         <v>8</v>
       </c>
-      <c r="BH45" s="222">
+      <c r="BH45" s="212">
         <v>8</v>
       </c>
-      <c r="BI45" s="223">
+      <c r="BI45" s="213">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
@@ -11311,16 +11308,16 @@
       <c r="BE46" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF46" s="211" t="s">
+      <c r="BF46" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="BG46" s="211">
+      <c r="BG46" s="201">
         <v>9</v>
       </c>
-      <c r="BH46" s="211">
+      <c r="BH46" s="201">
         <v>10</v>
       </c>
-      <c r="BI46" s="212">
+      <c r="BI46" s="202">
         <f t="shared" si="7"/>
         <v>9.5</v>
       </c>
@@ -11340,19 +11337,19 @@
       <c r="BD47" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE47" s="221" t="s">
+      <c r="BE47" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF47" s="222" t="s">
+      <c r="BF47" s="212" t="s">
         <v>16</v>
       </c>
-      <c r="BG47" s="222">
+      <c r="BG47" s="212">
         <v>11</v>
       </c>
-      <c r="BH47" s="222">
+      <c r="BH47" s="212">
         <v>16</v>
       </c>
-      <c r="BI47" s="223">
+      <c r="BI47" s="213">
         <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
@@ -11375,16 +11372,16 @@
       <c r="BE48" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF48" s="211" t="s">
+      <c r="BF48" s="201" t="s">
         <v>0</v>
       </c>
-      <c r="BG48" s="211">
+      <c r="BG48" s="201">
         <v>17</v>
       </c>
-      <c r="BH48" s="211">
+      <c r="BH48" s="201">
         <v>20</v>
       </c>
-      <c r="BI48" s="212">
+      <c r="BI48" s="202">
         <f t="shared" si="7"/>
         <v>18.5</v>
       </c>
@@ -11404,19 +11401,19 @@
       <c r="BD49" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE49" s="221" t="s">
+      <c r="BE49" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF49" s="222" t="s">
+      <c r="BF49" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="BG49" s="222">
+      <c r="BG49" s="212">
         <v>21</v>
       </c>
-      <c r="BH49" s="222">
+      <c r="BH49" s="212">
         <v>22</v>
       </c>
-      <c r="BI49" s="223">
+      <c r="BI49" s="213">
         <f t="shared" si="7"/>
         <v>21.5</v>
       </c>
@@ -11439,16 +11436,16 @@
       <c r="BE50" s="129" t="s">
         <v>61</v>
       </c>
-      <c r="BF50" s="213" t="s">
+      <c r="BF50" s="203" t="s">
         <v>17</v>
       </c>
-      <c r="BG50" s="213">
+      <c r="BG50" s="203">
         <v>1</v>
       </c>
-      <c r="BH50" s="213">
+      <c r="BH50" s="203">
         <v>4</v>
       </c>
-      <c r="BI50" s="214">
+      <c r="BI50" s="204">
         <f t="shared" si="7"/>
         <v>2.5</v>
       </c>
@@ -11468,19 +11465,19 @@
       <c r="BD51" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE51" s="221" t="s">
+      <c r="BE51" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF51" s="222" t="s">
+      <c r="BF51" s="212" t="s">
         <v>18</v>
       </c>
-      <c r="BG51" s="222">
+      <c r="BG51" s="212">
         <v>5</v>
       </c>
-      <c r="BH51" s="222">
+      <c r="BH51" s="212">
         <v>6</v>
       </c>
-      <c r="BI51" s="223">
+      <c r="BI51" s="213">
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
@@ -11503,16 +11500,16 @@
       <c r="BE52" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF52" s="211" t="s">
+      <c r="BF52" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="BG52" s="211">
+      <c r="BG52" s="201">
         <v>7</v>
       </c>
-      <c r="BH52" s="211">
+      <c r="BH52" s="201">
         <v>8</v>
       </c>
-      <c r="BI52" s="212">
+      <c r="BI52" s="202">
         <f t="shared" si="7"/>
         <v>7.5</v>
       </c>
@@ -11532,19 +11529,19 @@
       <c r="BD53" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE53" s="221" t="s">
+      <c r="BE53" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF53" s="222" t="s">
+      <c r="BF53" s="212" t="s">
         <v>20</v>
       </c>
-      <c r="BG53" s="222">
+      <c r="BG53" s="212">
         <v>9</v>
       </c>
-      <c r="BH53" s="222">
+      <c r="BH53" s="212">
         <v>10</v>
       </c>
-      <c r="BI53" s="223">
+      <c r="BI53" s="213">
         <f t="shared" si="7"/>
         <v>9.5</v>
       </c>
@@ -11567,16 +11564,16 @@
       <c r="BE54" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF54" s="211" t="s">
+      <c r="BF54" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="BG54" s="211">
+      <c r="BG54" s="201">
         <v>11</v>
       </c>
-      <c r="BH54" s="211">
+      <c r="BH54" s="201">
         <v>16</v>
       </c>
-      <c r="BI54" s="212">
+      <c r="BI54" s="202">
         <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
@@ -11585,19 +11582,19 @@
       <c r="BD55" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="BE55" s="221" t="s">
+      <c r="BE55" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF55" s="222" t="s">
+      <c r="BF55" s="212" t="s">
         <v>0</v>
       </c>
-      <c r="BG55" s="222">
+      <c r="BG55" s="212">
         <v>17</v>
       </c>
-      <c r="BH55" s="222">
+      <c r="BH55" s="212">
         <v>20</v>
       </c>
-      <c r="BI55" s="223">
+      <c r="BI55" s="213">
         <f t="shared" si="7"/>
         <v>18.5</v>
       </c>
@@ -11609,37 +11606,37 @@
       <c r="BE56" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="BF56" s="215" t="s">
+      <c r="BF56" s="205" t="s">
         <v>1</v>
       </c>
-      <c r="BG56" s="215">
+      <c r="BG56" s="205">
         <v>21</v>
       </c>
-      <c r="BH56" s="215">
+      <c r="BH56" s="205">
         <v>22</v>
       </c>
-      <c r="BI56" s="216">
+      <c r="BI56" s="206">
         <f t="shared" si="7"/>
         <v>21.5</v>
       </c>
     </row>
     <row r="57" spans="17:61" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="BD57" s="217" t="s">
+      <c r="BD57" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="BE57" s="218" t="s">
+      <c r="BE57" s="208" t="s">
         <v>60</v>
       </c>
-      <c r="BF57" s="219" t="s">
+      <c r="BF57" s="209" t="s">
         <v>136</v>
       </c>
-      <c r="BG57" s="219">
+      <c r="BG57" s="209">
         <v>1</v>
       </c>
-      <c r="BH57" s="219">
+      <c r="BH57" s="209">
         <v>3</v>
       </c>
-      <c r="BI57" s="220">
+      <c r="BI57" s="210">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
@@ -11651,16 +11648,16 @@
       <c r="BE58" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF58" s="211" t="s">
+      <c r="BF58" s="201" t="s">
         <v>137</v>
       </c>
-      <c r="BG58" s="211">
+      <c r="BG58" s="201">
         <v>4</v>
       </c>
-      <c r="BH58" s="211">
+      <c r="BH58" s="201">
         <v>5</v>
       </c>
-      <c r="BI58" s="212">
+      <c r="BI58" s="202">
         <f t="shared" si="7"/>
         <v>4.5</v>
       </c>
@@ -11669,19 +11666,19 @@
       <c r="BD59" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE59" s="221" t="s">
+      <c r="BE59" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF59" s="222" t="s">
+      <c r="BF59" s="212" t="s">
         <v>138</v>
       </c>
-      <c r="BG59" s="222">
+      <c r="BG59" s="212">
         <v>6</v>
       </c>
-      <c r="BH59" s="222">
+      <c r="BH59" s="212">
         <v>8</v>
       </c>
-      <c r="BI59" s="223">
+      <c r="BI59" s="213">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
@@ -11693,16 +11690,16 @@
       <c r="BE60" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF60" s="211" t="s">
+      <c r="BF60" s="201" t="s">
         <v>62</v>
       </c>
-      <c r="BG60" s="211">
+      <c r="BG60" s="201">
         <v>9</v>
       </c>
-      <c r="BH60" s="211">
+      <c r="BH60" s="201">
         <v>9</v>
       </c>
-      <c r="BI60" s="212">
+      <c r="BI60" s="202">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
@@ -11711,19 +11708,19 @@
       <c r="BD61" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE61" s="221" t="s">
+      <c r="BE61" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF61" s="222" t="s">
+      <c r="BF61" s="212" t="s">
         <v>63</v>
       </c>
-      <c r="BG61" s="222">
+      <c r="BG61" s="212">
         <v>10</v>
       </c>
-      <c r="BH61" s="222">
+      <c r="BH61" s="212">
         <v>10</v>
       </c>
-      <c r="BI61" s="223">
+      <c r="BI61" s="213">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
@@ -11735,16 +11732,16 @@
       <c r="BE62" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF62" s="211" t="s">
+      <c r="BF62" s="201" t="s">
         <v>45</v>
       </c>
-      <c r="BG62" s="211">
+      <c r="BG62" s="201">
         <v>11</v>
       </c>
-      <c r="BH62" s="211">
+      <c r="BH62" s="201">
         <v>11</v>
       </c>
-      <c r="BI62" s="212">
+      <c r="BI62" s="202">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
@@ -11753,19 +11750,19 @@
       <c r="BD63" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE63" s="221" t="s">
+      <c r="BE63" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF63" s="222" t="s">
+      <c r="BF63" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="BG63" s="222">
+      <c r="BG63" s="212">
         <v>12</v>
       </c>
-      <c r="BH63" s="222">
+      <c r="BH63" s="212">
         <v>15</v>
       </c>
-      <c r="BI63" s="223">
+      <c r="BI63" s="213">
         <f t="shared" si="7"/>
         <v>13.5</v>
       </c>
@@ -11777,16 +11774,16 @@
       <c r="BE64" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BF64" s="211" t="s">
+      <c r="BF64" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="BG64" s="211">
+      <c r="BG64" s="201">
         <v>16</v>
       </c>
-      <c r="BH64" s="211">
+      <c r="BH64" s="201">
         <v>21</v>
       </c>
-      <c r="BI64" s="212">
+      <c r="BI64" s="202">
         <f t="shared" si="7"/>
         <v>18.5</v>
       </c>
@@ -11795,19 +11792,19 @@
       <c r="BD65" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE65" s="221" t="s">
+      <c r="BE65" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="BF65" s="222" t="s">
+      <c r="BF65" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="BG65" s="222">
+      <c r="BG65" s="212">
         <v>22</v>
       </c>
-      <c r="BH65" s="222">
+      <c r="BH65" s="212">
         <v>22</v>
       </c>
-      <c r="BI65" s="223">
+      <c r="BI65" s="213">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
@@ -11819,16 +11816,16 @@
       <c r="BE66" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="BF66" s="213" t="s">
+      <c r="BF66" s="203" t="s">
         <v>136</v>
       </c>
-      <c r="BG66" s="213">
+      <c r="BG66" s="203">
         <v>1</v>
       </c>
-      <c r="BH66" s="213">
+      <c r="BH66" s="203">
         <v>2</v>
       </c>
-      <c r="BI66" s="214">
+      <c r="BI66" s="204">
         <f t="shared" si="7"/>
         <v>1.5</v>
       </c>
@@ -11837,19 +11834,19 @@
       <c r="BD67" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE67" s="221" t="s">
+      <c r="BE67" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF67" s="222" t="s">
+      <c r="BF67" s="212" t="s">
         <v>137</v>
       </c>
-      <c r="BG67" s="222">
+      <c r="BG67" s="212">
         <v>3</v>
       </c>
-      <c r="BH67" s="222">
+      <c r="BH67" s="212">
         <v>4</v>
       </c>
-      <c r="BI67" s="223">
+      <c r="BI67" s="213">
         <f t="shared" si="7"/>
         <v>3.5</v>
       </c>
@@ -11861,16 +11858,16 @@
       <c r="BE68" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF68" s="211" t="s">
+      <c r="BF68" s="201" t="s">
         <v>138</v>
       </c>
-      <c r="BG68" s="211">
+      <c r="BG68" s="201">
         <v>5</v>
       </c>
-      <c r="BH68" s="211">
+      <c r="BH68" s="201">
         <v>7</v>
       </c>
-      <c r="BI68" s="212">
+      <c r="BI68" s="202">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
@@ -11879,19 +11876,19 @@
       <c r="BD69" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE69" s="221" t="s">
+      <c r="BE69" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF69" s="222" t="s">
+      <c r="BF69" s="212" t="s">
         <v>62</v>
       </c>
-      <c r="BG69" s="222">
+      <c r="BG69" s="212">
         <v>8</v>
       </c>
-      <c r="BH69" s="222">
+      <c r="BH69" s="212">
         <v>8</v>
       </c>
-      <c r="BI69" s="223">
+      <c r="BI69" s="213">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
@@ -11903,16 +11900,16 @@
       <c r="BE70" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF70" s="211" t="s">
+      <c r="BF70" s="201" t="s">
         <v>63</v>
       </c>
-      <c r="BG70" s="211">
+      <c r="BG70" s="201">
         <v>9</v>
       </c>
-      <c r="BH70" s="211">
+      <c r="BH70" s="201">
         <v>9</v>
       </c>
-      <c r="BI70" s="212">
+      <c r="BI70" s="202">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
@@ -11921,19 +11918,19 @@
       <c r="BD71" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE71" s="221" t="s">
+      <c r="BE71" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF71" s="222" t="s">
-        <v>140</v>
-      </c>
-      <c r="BG71" s="222">
+      <c r="BF71" s="212" t="s">
+        <v>45</v>
+      </c>
+      <c r="BG71" s="212">
         <v>10</v>
       </c>
-      <c r="BH71" s="222">
+      <c r="BH71" s="212">
         <v>10</v>
       </c>
-      <c r="BI71" s="223">
+      <c r="BI71" s="213">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
@@ -11945,16 +11942,16 @@
       <c r="BE72" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF72" s="211" t="s">
+      <c r="BF72" s="201" t="s">
         <v>42</v>
       </c>
-      <c r="BG72" s="211">
+      <c r="BG72" s="201">
         <v>11</v>
       </c>
-      <c r="BH72" s="211">
+      <c r="BH72" s="201">
         <v>14</v>
       </c>
-      <c r="BI72" s="212">
+      <c r="BI72" s="202">
         <f t="shared" si="7"/>
         <v>12.5</v>
       </c>
@@ -11963,19 +11960,19 @@
       <c r="BD73" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE73" s="221" t="s">
+      <c r="BE73" s="211" t="s">
         <v>70</v>
       </c>
-      <c r="BF73" s="222" t="s">
+      <c r="BF73" s="212" t="s">
         <v>43</v>
       </c>
-      <c r="BG73" s="222">
+      <c r="BG73" s="212">
         <v>15</v>
       </c>
-      <c r="BH73" s="222">
+      <c r="BH73" s="212">
         <v>21</v>
       </c>
-      <c r="BI73" s="223">
+      <c r="BI73" s="213">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
@@ -11987,37 +11984,37 @@
       <c r="BE74" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="BF74" s="211" t="s">
+      <c r="BF74" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="BG74" s="211">
+      <c r="BG74" s="201">
         <v>22</v>
       </c>
-      <c r="BH74" s="211">
+      <c r="BH74" s="201">
         <v>22</v>
       </c>
-      <c r="BI74" s="212">
+      <c r="BI74" s="202">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
     </row>
     <row r="75" spans="56:61" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="BD75" s="224" t="s">
+      <c r="BD75" s="214" t="s">
         <v>11</v>
       </c>
-      <c r="BE75" s="225" t="s">
+      <c r="BE75" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="BF75" s="226" t="s">
+      <c r="BF75" s="216" t="s">
         <v>136</v>
       </c>
-      <c r="BG75" s="226">
+      <c r="BG75" s="216">
         <v>1</v>
       </c>
-      <c r="BH75" s="226">
+      <c r="BH75" s="216">
         <v>1</v>
       </c>
-      <c r="BI75" s="227">
+      <c r="BI75" s="217">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
@@ -12029,16 +12026,16 @@
       <c r="BE76" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF76" s="211" t="s">
+      <c r="BF76" s="201" t="s">
         <v>137</v>
       </c>
-      <c r="BG76" s="211">
+      <c r="BG76" s="201">
         <v>2</v>
       </c>
-      <c r="BH76" s="211">
+      <c r="BH76" s="201">
         <v>3</v>
       </c>
-      <c r="BI76" s="212">
+      <c r="BI76" s="202">
         <f t="shared" ref="BI76:BI83" si="10">AVERAGE(BG76:BH76)</f>
         <v>2.5</v>
       </c>
@@ -12047,19 +12044,19 @@
       <c r="BD77" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE77" s="221" t="s">
+      <c r="BE77" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF77" s="222" t="s">
+      <c r="BF77" s="212" t="s">
         <v>138</v>
       </c>
-      <c r="BG77" s="222">
+      <c r="BG77" s="212">
         <v>4</v>
       </c>
-      <c r="BH77" s="222">
+      <c r="BH77" s="212">
         <v>6</v>
       </c>
-      <c r="BI77" s="223">
+      <c r="BI77" s="213">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
@@ -12071,16 +12068,16 @@
       <c r="BE78" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF78" s="211" t="s">
+      <c r="BF78" s="201" t="s">
         <v>62</v>
       </c>
-      <c r="BG78" s="211">
+      <c r="BG78" s="201">
         <v>7</v>
       </c>
-      <c r="BH78" s="211">
+      <c r="BH78" s="201">
         <v>8</v>
       </c>
-      <c r="BI78" s="212">
+      <c r="BI78" s="202">
         <f t="shared" si="10"/>
         <v>7.5</v>
       </c>
@@ -12089,19 +12086,19 @@
       <c r="BD79" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE79" s="221" t="s">
+      <c r="BE79" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF79" s="222" t="s">
+      <c r="BF79" s="212" t="s">
         <v>63</v>
       </c>
-      <c r="BG79" s="222">
+      <c r="BG79" s="212">
         <v>9</v>
       </c>
-      <c r="BH79" s="222">
+      <c r="BH79" s="212">
         <v>9</v>
       </c>
-      <c r="BI79" s="223">
+      <c r="BI79" s="213">
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
@@ -12113,16 +12110,16 @@
       <c r="BE80" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF80" s="211" t="s">
+      <c r="BF80" s="201" t="s">
         <v>45</v>
       </c>
-      <c r="BG80" s="211">
+      <c r="BG80" s="201">
         <v>10</v>
       </c>
-      <c r="BH80" s="211">
+      <c r="BH80" s="201">
         <v>10</v>
       </c>
-      <c r="BI80" s="212">
+      <c r="BI80" s="202">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
@@ -12131,19 +12128,19 @@
       <c r="BD81" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="BE81" s="221" t="s">
+      <c r="BE81" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="BF81" s="222" t="s">
+      <c r="BF81" s="212" t="s">
         <v>42</v>
       </c>
-      <c r="BG81" s="222">
+      <c r="BG81" s="212">
         <v>11</v>
       </c>
-      <c r="BH81" s="222">
+      <c r="BH81" s="212">
         <v>14</v>
       </c>
-      <c r="BI81" s="223">
+      <c r="BI81" s="213">
         <f t="shared" si="10"/>
         <v>12.5</v>
       </c>
@@ -12155,37 +12152,37 @@
       <c r="BE82" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BF82" s="211" t="s">
+      <c r="BF82" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="BG82" s="211">
+      <c r="BG82" s="201">
         <v>15</v>
       </c>
-      <c r="BH82" s="211">
+      <c r="BH82" s="201">
         <v>21</v>
       </c>
-      <c r="BI82" s="212">
+      <c r="BI82" s="202">
         <f t="shared" si="10"/>
         <v>18</v>
       </c>
     </row>
     <row r="83" spans="56:61" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="BD83" s="229" t="s">
+      <c r="BD83" s="219" t="s">
         <v>11</v>
       </c>
-      <c r="BE83" s="230" t="s">
+      <c r="BE83" s="220" t="s">
         <v>61</v>
       </c>
-      <c r="BF83" s="231" t="s">
+      <c r="BF83" s="221" t="s">
         <v>1</v>
       </c>
-      <c r="BG83" s="231">
+      <c r="BG83" s="221">
         <v>22</v>
       </c>
-      <c r="BH83" s="231">
+      <c r="BH83" s="221">
         <v>22</v>
       </c>
-      <c r="BI83" s="232">
+      <c r="BI83" s="222">
         <f t="shared" si="10"/>
         <v>22</v>
       </c>

</xml_diff>